<commit_message>
Small edit to edited-species5.csv again
</commit_message>
<xml_diff>
--- a/data/raw/intermediate-dependency2-edited_conflicting-monitoring-info-resolved.xlsx
+++ b/data/raw/intermediate-dependency2-edited_conflicting-monitoring-info-resolved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{47F7A776-7B70-4FE9-9FFA-A12BF92F7459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{52686497-AA3E-4292-A5A5-7F6395E8BE04}"/>
+  <xr:revisionPtr revIDLastSave="153" documentId="8_{47F7A776-7B70-4FE9-9FFA-A12BF92F7459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6BABB8EF-838D-488F-9521-FB0050DD8FF1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="12408" windowHeight="8892" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comparison" sheetId="1" r:id="rId1"/>
@@ -1559,8 +1559,8 @@
   <dimension ref="A1:N244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>